<commit_message>
Fixed sensor data extraction
</commit_message>
<xml_diff>
--- a/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
+++ b/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>unsatisfied_condition_description</t>
+          <t>process_model_id</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,67 +460,67 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>complete_service_time</t>
+          <t>response_status_code</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>SubProcessID</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>dict</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>response_status_code</t>
+          <t>case</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>human_workstation_green_button_pressed</t>
+          <t>complete_service_time</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>time:timestamp</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>dict</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>process_model_id</t>
+          <t>lifecycle:transition</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,19 +532,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SubProcessID</t>
+          <t>human_workstation_green_button_pressed</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>case</t>
+          <t>org:resource</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>case:concept:name</t>
+          <t>requested_service_url</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,19 +568,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>operation_end_time</t>
+          <t>lifecycle:state</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>requested_service_url</t>
+          <t>identifier:id</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,7 +592,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>org:resource</t>
+          <t>current_task</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,7 +604,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>concept:name</t>
+          <t>event_id</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -616,7 +616,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>lifecycle:state</t>
+          <t>unsatisfied_condition_description</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -628,7 +628,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>current_task</t>
+          <t>case:concept:name</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -640,7 +640,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>event_id</t>
+          <t>concept:name</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -664,24 +664,24 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>lifecycle:transition</t>
+          <t>operation_end_time</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>identifier:id</t>
+          <t>time:timestamp</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
With combined sensor data file
</commit_message>
<xml_diff>
--- a/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
+++ b/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>process_model_id</t>
+          <t>concept:name</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,19 +460,19 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>response_status_code</t>
+          <t>operation_end_time</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SubProcessID</t>
+          <t>lifecycle:transition</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,7 +484,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>case</t>
+          <t>current_task</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -508,19 +508,19 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>time:timestamp</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>dict</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>lifecycle:transition</t>
+          <t>process_model_id</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,19 +532,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>human_workstation_green_button_pressed</t>
+          <t>planned_operation_time</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>org:resource</t>
+          <t>SubProcessID</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>requested_service_url</t>
+          <t>case:concept:name</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>lifecycle:state</t>
+          <t>case</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -592,7 +592,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>current_task</t>
+          <t>requested_service_url</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,12 +604,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>event_id</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>dict</t>
         </is>
       </c>
     </row>
@@ -628,7 +628,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>case:concept:name</t>
+          <t>org:resource</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -640,19 +640,19 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>concept:name</t>
+          <t>response_status_code</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>planned_operation_time</t>
+          <t>event_id</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,24 +664,24 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>operation_end_time</t>
+          <t>human_workstation_green_button_pressed</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>time:timestamp</t>
+          <t>lifecycle:state</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Store all trace and event attributes (for cleaned event log file)
</commit_message>
<xml_diff>
--- a/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
+++ b/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>lifecycle:transition</t>
+          <t>planned_operation_time</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>case</t>
+          <t>requested_service_url</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,19 +472,19 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>response_status_code</t>
+          <t>time:timestamp</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>concept:name</t>
+          <t>SubProcessID</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,31 +496,31 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>time:timestamp</t>
+          <t>unsatisfied_condition_description</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>planned_operation_time</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>dict</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>case:concept:name</t>
+          <t>lifecycle:transition</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>unsatisfied_condition_description</t>
+          <t>org:resource</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,19 +544,19 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>human_workstation_green_button_pressed</t>
+          <t>lifecycle:state</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SubProcessID</t>
+          <t>case:concept:name</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,19 +568,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>lifecycle:state</t>
+          <t>operation_end_time</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>process_model_id</t>
+          <t>complete_service_time</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,31 +592,31 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>operation_end_time</t>
+          <t>current_task</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>human_workstation_green_button_pressed</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>dict</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>requested_service_url</t>
+          <t>event_id</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -628,19 +628,19 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>current_task</t>
+          <t>response_status_code</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>event_id</t>
+          <t>concept:name</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>identifier:id</t>
+          <t>case</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>complete_service_time</t>
+          <t>identifier:id</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>org:resource</t>
+          <t>process_model_id</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">

</xml_diff>

<commit_message>
Fixed sensor data loading (ram issue) and changes in jupyter notebook
</commit_message>
<xml_diff>
--- a/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
+++ b/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>planned_operation_time</t>
+          <t>case</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,43 +460,43 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>requested_service_url</t>
+          <t>human_workstation_green_button_pressed</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>time:timestamp</t>
+          <t>lifecycle:state</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SubProcessID</t>
+          <t>operation_end_time</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>unsatisfied_condition_description</t>
+          <t>complete_service_time</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,19 +508,19 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>identifier:id</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>dict</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>lifecycle:transition</t>
+          <t>process_model_id</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>org:resource</t>
+          <t>concept:name</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>lifecycle:state</t>
+          <t>requested_service_url</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -568,19 +568,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>operation_end_time</t>
+          <t>unsatisfied_condition_description</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>complete_service_time</t>
+          <t>lifecycle:transition</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,7 +592,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>current_task</t>
+          <t>planned_operation_time</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,19 +604,19 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>human_workstation_green_button_pressed</t>
+          <t>event_id</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>event_id</t>
+          <t>SubProcessID</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -628,19 +628,19 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>response_status_code</t>
+          <t>org:resource</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>concept:name</t>
+          <t>current_task</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,36 +652,36 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>case</t>
+          <t>time:timestamp</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>identifier:id</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>dict</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>process_model_id</t>
+          <t>response_status_code</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Number of rows in sensor data no longer shown in query
</commit_message>
<xml_diff>
--- a/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
+++ b/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>case</t>
+          <t>lifecycle:transition</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,19 +460,19 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>human_workstation_green_button_pressed</t>
+          <t>time:timestamp</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>lifecycle:state</t>
+          <t>case</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,19 +484,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>operation_end_time</t>
+          <t>complete_service_time</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>complete_service_time</t>
+          <t>identifier:id</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>identifier:id</t>
+          <t>unsatisfied_condition_description</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,31 +520,31 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>process_model_id</t>
+          <t>human_workstation_green_button_pressed</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>concept:name</t>
+          <t>response_status_code</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>requested_service_url</t>
+          <t>concept:name</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>case:concept:name</t>
+          <t>SubProcessID</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>unsatisfied_condition_description</t>
+          <t>lifecycle:state</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>lifecycle:transition</t>
+          <t>planned_operation_time</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,7 +592,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>planned_operation_time</t>
+          <t>process_model_id</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,7 +604,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>event_id</t>
+          <t>current_task</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -616,7 +616,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SubProcessID</t>
+          <t>org:resource</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -628,19 +628,19 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>org:resource</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>dict</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>current_task</t>
+          <t>case:concept:name</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>time:timestamp</t>
+          <t>operation_end_time</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,24 +664,24 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>requested_service_url</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>dict</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>response_status_code</t>
+          <t>event_id</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Grouping in dfg detection
</commit_message>
<xml_diff>
--- a/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
+++ b/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
@@ -448,31 +448,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>human_workstation_green_button_pressed</t>
+          <t>current_task</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>requested_service_url</t>
+          <t>time:timestamp</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>current_task</t>
+          <t>complete_service_time</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,7 +484,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>unsatisfied_condition_description</t>
+          <t>SubProcessID</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,43 +496,43 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>case:concept:name</t>
+          <t>response_status_code</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>case</t>
+          <t>human_workstation_green_button_pressed</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>operation_end_time</t>
+          <t>org:resource</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>lifecycle:state</t>
+          <t>identifier:id</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>event_id</t>
+          <t>process_model_id</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>process_model_id</t>
+          <t>lifecycle:state</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,19 +568,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>time:timestamp</t>
+          <t>lifecycle:transition</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>concept:name</t>
+          <t>case</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,43 +592,43 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>identifier:id</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>dict</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>planned_operation_time</t>
+          <t>operation_end_time</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>response_status_code</t>
+          <t>unsatisfied_condition_description</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>lifecycle:transition</t>
+          <t>event_id</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -640,7 +640,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>org:resource</t>
+          <t>case:concept:name</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>complete_service_time</t>
+          <t>planned_operation_time</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,19 +664,19 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>requested_service_url</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>dict</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SubProcessID</t>
+          <t>concept:name</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">

</xml_diff>

<commit_message>
Added sensordata frequency checking
</commit_message>
<xml_diff>
--- a/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
+++ b/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
@@ -460,19 +460,19 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>time:timestamp</t>
+          <t>case:concept:name</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>complete_service_time</t>
+          <t>org:resource</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,19 +484,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SubProcessID</t>
+          <t>response_status_code</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>response_status_code</t>
+          <t>human_workstation_green_button_pressed</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,19 +508,19 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>human_workstation_green_button_pressed</t>
+          <t>identifier:id</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>org:resource</t>
+          <t>lifecycle:state</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>identifier:id</t>
+          <t>unsatisfied_condition_description</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,19 +544,19 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>process_model_id</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>dict</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>lifecycle:state</t>
+          <t>event_id</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>lifecycle:transition</t>
+          <t>planned_operation_time</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>case</t>
+          <t>complete_service_time</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,12 +592,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>process_model_id</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>dict</t>
+          <t>str</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>unsatisfied_condition_description</t>
+          <t>SubProcessID</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -628,19 +628,19 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>event_id</t>
+          <t>time:timestamp</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>case:concept:name</t>
+          <t>requested_service_url</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>planned_operation_time</t>
+          <t>lifecycle:transition</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>requested_service_url</t>
+          <t>case</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">

</xml_diff>

<commit_message>
Finnished synthetic data creation
</commit_message>
<xml_diff>
--- a/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
+++ b/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>current_task</t>
+          <t>case:concept:name</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>case:concept:name</t>
+          <t>requested_service_url</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,31 +472,31 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>org:resource</t>
+          <t>human_workstation_green_button_pressed</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>response_status_code</t>
+          <t>lifecycle:state</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>human_workstation_green_button_pressed</t>
+          <t>response_status_code</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>identifier:id</t>
+          <t>process_model_id</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,43 +520,43 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>lifecycle:state</t>
+          <t>operation_end_time</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>unsatisfied_condition_description</t>
+          <t>time:timestamp</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>org:resource</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>dict</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>event_id</t>
+          <t>planned_operation_time</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,19 +568,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>planned_operation_time</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>dict</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>complete_service_time</t>
+          <t>unsatisfied_condition_description</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,7 +592,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>process_model_id</t>
+          <t>event_id</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,19 +604,19 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>operation_end_time</t>
+          <t>SubProcessID</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SubProcessID</t>
+          <t>complete_service_time</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -628,19 +628,19 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>time:timestamp</t>
+          <t>current_task</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>requested_service_url</t>
+          <t>concept:name</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>lifecycle:transition</t>
+          <t>case</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>case</t>
+          <t>lifecycle:transition</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>concept:name</t>
+          <t>identifier:id</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">

</xml_diff>

<commit_message>
Finnished synthetic data creation for pressure sensor
</commit_message>
<xml_diff>
--- a/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
+++ b/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>case:concept:name</t>
+          <t>concept:name</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>requested_service_url</t>
+          <t>case:concept:name</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,19 +472,19 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>human_workstation_green_button_pressed</t>
+          <t>lifecycle:state</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>lifecycle:state</t>
+          <t>unsatisfied_condition_description</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -508,43 +508,43 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>process_model_id</t>
+          <t>time:timestamp</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>operation_end_time</t>
+          <t>identifier:id</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>time:timestamp</t>
+          <t>planned_operation_time</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>org:resource</t>
+          <t>complete_service_time</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>planned_operation_time</t>
+          <t>event_id</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,19 +568,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>SubProcessID</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>dict</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>unsatisfied_condition_description</t>
+          <t>process_model_id</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,7 +592,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>event_id</t>
+          <t>org:resource</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,19 +604,19 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>SubProcessID</t>
+          <t>operation_end_time</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>complete_service_time</t>
+          <t>lifecycle:transition</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -628,19 +628,19 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>current_task</t>
+          <t>human_workstation_green_button_pressed</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>concept:name</t>
+          <t>requested_service_url</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>lifecycle:transition</t>
+          <t>current_task</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -676,12 +676,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>identifier:id</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>dict</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added calculation of number of processes per resource
</commit_message>
<xml_diff>
--- a/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
+++ b/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>event_id</t>
+          <t>requested_service_url</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,19 +472,19 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>concept:name</t>
+          <t>operation_end_time</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SubProcessID</t>
+          <t>lifecycle:transition</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>lifecycle:transition</t>
+          <t>complete_service_time</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,31 +508,31 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>requested_service_url</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>dict</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>time:timestamp</t>
+          <t>case:concept:name</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>case</t>
+          <t>concept:name</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>case:concept:name</t>
+          <t>org:resource</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,19 +556,19 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>human_workstation_green_button_pressed</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>dict</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>identifier:id</t>
+          <t>unsatisfied_condition_description</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -580,19 +580,19 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>human_workstation_green_button_pressed</t>
+          <t>process_model_id</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>current_task</t>
+          <t>case</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,7 +604,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>process_model_id</t>
+          <t>SubProcessID</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -616,31 +616,31 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>unsatisfied_condition_description</t>
+          <t>time:timestamp</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>operation_end_time</t>
+          <t>identifier:id</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>lifecycle:state</t>
+          <t>event_id</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>org:resource</t>
+          <t>current_task</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>complete_service_time</t>
+          <t>lifecycle:state</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">

</xml_diff>

<commit_message>
Removed "elapsed_seconds_since_start" form autoencoder test due to non existance
</commit_message>
<xml_diff>
--- a/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
+++ b/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
@@ -448,19 +448,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>planned_operation_time</t>
+          <t>operation_end_time</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>requested_service_url</t>
+          <t>SubProcessID</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,19 +472,19 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>operation_end_time</t>
+          <t>case</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>lifecycle:transition</t>
+          <t>identifier:id</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>complete_service_time</t>
+          <t>org:resource</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,43 +508,43 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>complete_service_time</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>dict</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>case:concept:name</t>
+          <t>human_workstation_green_button_pressed</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>concept:name</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>dict</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>org:resource</t>
+          <t>concept:name</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,31 +556,31 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>human_workstation_green_button_pressed</t>
+          <t>lifecycle:transition</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>unsatisfied_condition_description</t>
+          <t>response_status_code</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>process_model_id</t>
+          <t>case:concept:name</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,19 +592,19 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>case</t>
+          <t>time:timestamp</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>SubProcessID</t>
+          <t>unsatisfied_condition_description</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -616,19 +616,19 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>time:timestamp</t>
+          <t>process_model_id</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>identifier:id</t>
+          <t>lifecycle:state</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -640,7 +640,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>event_id</t>
+          <t>current_task</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>current_task</t>
+          <t>planned_operation_time</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>lifecycle:state</t>
+          <t>event_id</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -676,12 +676,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>response_status_code</t>
+          <t>requested_service_url</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Partially finnished ae implementation
</commit_message>
<xml_diff>
--- a/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
+++ b/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
@@ -448,43 +448,43 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>lifecycle:transition</t>
+          <t>operation_end_time</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SubProcessID</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>dict</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>response_status_code</t>
+          <t>SubProcessID</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>event_id</t>
+          <t>identifier:id</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>concept:name</t>
+          <t>lifecycle:transition</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>process_model_id</t>
+          <t>complete_service_time</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,7 +520,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>current_task</t>
+          <t>concept:name</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,19 +532,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>operation_end_time</t>
+          <t>process_model_id</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>case</t>
+          <t>event_id</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>complete_service_time</t>
+          <t>case</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,19 +568,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>org:resource</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>dict</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>case:concept:name</t>
+          <t>requested_service_url</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,7 +592,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>human_workstation_green_button_pressed</t>
+          <t>response_status_code</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,7 +604,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>identifier:id</t>
+          <t>unsatisfied_condition_description</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -616,12 +616,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>requested_service_url</t>
+          <t>human_workstation_green_button_pressed</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>org:resource</t>
+          <t>planned_operation_time</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>planned_operation_time</t>
+          <t>lifecycle:state</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>unsatisfied_condition_description</t>
+          <t>case:concept:name</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>lifecycle:state</t>
+          <t>current_task</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">

</xml_diff>

<commit_message>
added anomaly detection file + small changes
</commit_message>
<xml_diff>
--- a/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
+++ b/Data/IoT enriched event log paper/tables/main_event_attribute_info.xlsx
@@ -448,31 +448,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>operation_end_time</t>
+          <t>case</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>parameters</t>
+          <t>operation_end_time</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>dict</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SubProcessID</t>
+          <t>case:concept:name</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,7 +484,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>identifier:id</t>
+          <t>event_id</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>lifecycle:transition</t>
+          <t>lifecycle:state</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,43 +508,43 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>complete_service_time</t>
+          <t>time:timestamp</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>datetime</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>concept:name</t>
+          <t>human_workstation_green_button_pressed</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>process_model_id</t>
+          <t>parameters</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>dict</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>event_id</t>
+          <t>identifier:id</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>case</t>
+          <t>process_model_id</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>org:resource</t>
+          <t>requested_service_url</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>requested_service_url</t>
+          <t>concept:name</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,55 +592,55 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>response_status_code</t>
+          <t>current_task</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>unsatisfied_condition_description</t>
+          <t>response_status_code</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>float</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>human_workstation_green_button_pressed</t>
+          <t>org:resource</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>float</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>time:timestamp</t>
+          <t>unsatisfied_condition_description</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>str</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>planned_operation_time</t>
+          <t>lifecycle:transition</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>lifecycle:state</t>
+          <t>complete_service_time</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>case:concept:name</t>
+          <t>SubProcessID</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>current_task</t>
+          <t>planned_operation_time</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">

</xml_diff>